<commit_message>
Updated Sprint 3 Documentation
</commit_message>
<xml_diff>
--- a/documentation/Sprint 3/Sprint 3 Retrospective.xlsx
+++ b/documentation/Sprint 3/Sprint 3 Retrospective.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25217"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jig13\source\repos\Tracr\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B9FAA56-0689-4AEF-AA0C-0BEED3DD7BF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{6B9FAA56-0689-4AEF-AA0C-0BEED3DD7BF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DB8E19AD-2EA2-48E9-9D55-27FE3D4B4370}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15225" xr2:uid="{72CB5AE4-9E8C-466B-B4FC-F83356BD9814}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sprint (number)" sheetId="1" r:id="rId1"/>
+    <sheet name="Sprint 3" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -27,6 +27,7 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>What should we start doing?</t>
   </si>
@@ -44,12 +45,21 @@
   <si>
     <t>What should we continue doing?</t>
   </si>
+  <si>
+    <t>Team should begin working on Final Presentation for the Final Project deliverable</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>N.A</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -66,6 +76,11 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -89,7 +104,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -99,6 +114,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -414,13 +432,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DE5DFCB-F97B-4E90-B6F9-D1CAF5115B15}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="52.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="35.140625" style="1" customWidth="1"/>
@@ -428,7 +446,7 @@
     <col min="4" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15.75">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -439,7 +457,229 @@
         <v>2</v>
       </c>
     </row>
+    <row r="2" spans="1:3" ht="30">
+      <c r="A2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000B81FB27D8318F409DB8592A1F03A407" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="dd4a8a8bedfbf32d1389488a2d4ed985">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="fd8108f1-5f5d-4cb7-bb4b-e2aea97cbd6a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6fab11e5e5165e332b604d13f2f72455" ns2:_="">
+    <xsd:import namespace="fd8108f1-5f5d-4cb7-bb4b-e2aea97cbd6a"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="fd8108f1-5f5d-4cb7-bb4b-e2aea97cbd6a" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="10" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceKeyPoints" ma:index="11" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoTags" ma:index="12" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="13" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="14" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="15" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="16" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="17" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C03A529-983D-4361-8FAF-CE09FB6F2BB5}"/>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{45A4EFD3-1A35-4176-A2AD-AF47B99943DE}"/>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A21CFD8C-CFFC-4244-8F04-2592D80D1A8B}"/>
 </file>
</xml_diff>